<commit_message>
New Player totals table
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\documents\random\TheFarmingGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1240FB8A-E4E1-475E-934E-71953472D99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D29E19-9F6C-4BE2-A755-38A4B459C529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{E5385B3E-3C09-4B0C-AE62-752D26427E58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{E5385B3E-3C09-4B0C-AE62-752D26427E58}"/>
   </bookViews>
   <sheets>
     <sheet name="Board" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="194">
   <si>
     <t>Card</t>
   </si>
@@ -565,6 +565,63 @@
   </si>
   <si>
     <t>Fourth-Hay-Cutting</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Net Worth</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Debt</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Livestock</t>
+  </si>
+  <si>
+    <t>Hay</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>Ahtanum</t>
+  </si>
+  <si>
+    <t>Rattle</t>
+  </si>
+  <si>
+    <t>Casade</t>
+  </si>
+  <si>
+    <t>Toppenish</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Tractors</t>
+  </si>
+  <si>
+    <t>Harvester</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>other name</t>
   </si>
 </sst>
 </file>
@@ -608,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -621,6 +678,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2163,53 +2223,166 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28CB90E-5B61-4A99-B273-6F078CDD9FA6}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>104</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C11:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2357,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365E4D37-5863-4017-8DB4-DB9D3279A2C3}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>